<commit_message>
frontend-backend integration, but obj is 10087 for some reason
</commit_message>
<xml_diff>
--- a/output_qualtrics.xlsx
+++ b/output_qualtrics.xlsx
@@ -55,112 +55,112 @@
     <t>5-6 PM</t>
   </si>
   <si>
-    <t>['Name 19', 'Name 9']</t>
-  </si>
-  <si>
-    <t>['Name 13', 'Name 17']</t>
-  </si>
-  <si>
-    <t>['Name 17', 'Name 40']</t>
-  </si>
-  <si>
-    <t>['Name 18', 'Name 6']</t>
-  </si>
-  <si>
-    <t>['Name 25', 'Name 39']</t>
-  </si>
-  <si>
-    <t>['Name 16', 'Name 25']</t>
-  </si>
-  <si>
-    <t>['Name 25', 'Name 28']</t>
-  </si>
-  <si>
-    <t>['Name 34', 'Name 41']</t>
-  </si>
-  <si>
-    <t>['Name 30', 'Name 42']</t>
-  </si>
-  <si>
-    <t>['Name 22', 'Name 43']</t>
-  </si>
-  <si>
-    <t>['Name 19', 'Name 40']</t>
-  </si>
-  <si>
-    <t>['Name 27', 'Name 35']</t>
-  </si>
-  <si>
-    <t>['Name 11', 'Name 33']</t>
-  </si>
-  <si>
-    <t>['Name I', 'Name 18']</t>
-  </si>
-  <si>
-    <t>['Name 30', 'Name 41']</t>
-  </si>
-  <si>
-    <t>['Name 23', 'Name 37']</t>
-  </si>
-  <si>
-    <t>['Name 3', 'Name 7']</t>
-  </si>
-  <si>
-    <t>['Name 2', 'Name 13']</t>
-  </si>
-  <si>
-    <t>['Name 36', 'Name 6']</t>
-  </si>
-  <si>
-    <t>['Name 27', 'Name 38']</t>
-  </si>
-  <si>
-    <t>['Name 20', 'Name 40']</t>
-  </si>
-  <si>
-    <t>['Name 31', 'Name 5']</t>
-  </si>
-  <si>
-    <t>['Name 23', 'Name 35']</t>
-  </si>
-  <si>
-    <t>['Name I', 'Name 41']</t>
-  </si>
-  <si>
-    <t>['Name 21', 'Name 42']</t>
-  </si>
-  <si>
-    <t>['Name 26', 'Name 43']</t>
-  </si>
-  <si>
-    <t>['Name 15', 'Name 29']</t>
-  </si>
-  <si>
-    <t>['Name 2', 'Name 4']</t>
-  </si>
-  <si>
-    <t>['Name 16', 'Name 5']</t>
-  </si>
-  <si>
-    <t>['Name 12', 'Name 33']</t>
-  </si>
-  <si>
-    <t>['Name 12', 'Name 38']</t>
-  </si>
-  <si>
-    <t>['Name 5', 'Name 10']</t>
-  </si>
-  <si>
-    <t>['Name 32', 'Name 9']</t>
-  </si>
-  <si>
-    <t>['Name 20', 'Name 26']</t>
-  </si>
-  <si>
-    <t>['Name 24', 'Name 8']</t>
-  </si>
-  <si>
-    <t>['Name 14', 'Name 31']</t>
+    <t>['Taya Yakovenko', 'Aidan James Cook ']</t>
+  </si>
+  <si>
+    <t>['Hannah Peloquin', 'Daniel Sardak']</t>
+  </si>
+  <si>
+    <t>['Sarah Roberge', 'Dhruv Chheda']</t>
+  </si>
+  <si>
+    <t>['Peiyao Lai', 'Dane Johnson']</t>
+  </si>
+  <si>
+    <t>['Darcy Milligan', 'Jeel Chatrola']</t>
+  </si>
+  <si>
+    <t>['Rosaline Guo', 'Jeel Chatrola']</t>
+  </si>
+  <si>
+    <t>['Zixiao Chen', 'Cameron James Norton']</t>
+  </si>
+  <si>
+    <t>['Zixiao Chen', 'Thira Patel']</t>
+  </si>
+  <si>
+    <t>['Ethan Lima', 'Jeel Chatrola']</t>
+  </si>
+  <si>
+    <t>['Hammed Olayinka', 'Jeel Chatrola']</t>
+  </si>
+  <si>
+    <t>['Hammed Olayinka', 'Xiaoyu Chen']</t>
+  </si>
+  <si>
+    <t>['zihang xu', 'Jeel Chatrola']</t>
+  </si>
+  <si>
+    <t>['Yulong Jiang', 'Nicholas Shannon']</t>
+  </si>
+  <si>
+    <t>['Peiyao Lai', 'Evan Sayer']</t>
+  </si>
+  <si>
+    <t>['Dashiell Elliott', 'Rholee Xu']</t>
+  </si>
+  <si>
+    <t>['Tony Vuolo', 'Rholee Xu']</t>
+  </si>
+  <si>
+    <t>['Abigail Rose Lindner', 'Sara Amato']</t>
+  </si>
+  <si>
+    <t>['Grace Cao', 'Xiaoyu Chen']</t>
+  </si>
+  <si>
+    <t>['Sophia Kouznetsov', 'Jeel Chatrola']</t>
+  </si>
+  <si>
+    <t>['Sycamore Herlihy', 'Bailey Allmon']</t>
+  </si>
+  <si>
+    <t>['Tony Vuolo', 'Dane Johnson']</t>
+  </si>
+  <si>
+    <t>['Yulong Jiang', 'Thira Patel']</t>
+  </si>
+  <si>
+    <t>['zihang xu', 'Andrey Martemyanov ']</t>
+  </si>
+  <si>
+    <t>['Lingli Yang', 'Andrey Martemyanov ']</t>
+  </si>
+  <si>
+    <t>['Abigail Rose Lindner', 'Lauren Braconnier ']</t>
+  </si>
+  <si>
+    <t>['Natalie Tierney', 'Caitlin Murphy']</t>
+  </si>
+  <si>
+    <t>['Duyen Le', 'Om Vinayak Gaikwad']</t>
+  </si>
+  <si>
+    <t>['Teodor Hellgren', 'Devin Roskoph']</t>
+  </si>
+  <si>
+    <t>['Alex Tomellini', 'Evan Sayer']</t>
+  </si>
+  <si>
+    <t>['Wyatt Binnard', 'Kevin Metzler']</t>
+  </si>
+  <si>
+    <t>['Kevin Metzler', 'Elizabeth Bowman']</t>
+  </si>
+  <si>
+    <t>['Ngoc Pham', 'Om Vinayak Gaikwad']</t>
+  </si>
+  <si>
+    <t>['Minh Bui', 'Sara Amato']</t>
+  </si>
+  <si>
+    <t>['Mena Youssif', 'Navpreet Kaur']</t>
+  </si>
+  <si>
+    <t>['William Folan', 'Avery Rabidoux']</t>
+  </si>
+  <si>
+    <t>['Lingli Yang', 'Thira Patel']</t>
   </si>
   <si>
     <t>[]</t>

</xml_diff>